<commit_message>
added fund_name as var
</commit_message>
<xml_diff>
--- a/reporting_fund/fund_template.xlsx
+++ b/reporting_fund/fund_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Felix/DEV/xlwings-demo/reporting_fund/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{995DEB3F-3127-4941-9E95-8C8567096C0B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEFEDD60-11EF-9741-8ADF-4702171C475F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-5140" yWindow="-21140" windowWidth="38400" windowHeight="21140" xr2:uid="{2269DA39-2FA8-EE4B-884F-E4AE05C32F51}"/>
   </bookViews>
@@ -40,9 +40,6 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="67">
-  <si>
-    <t>xlwings Fund</t>
-  </si>
   <si>
     <t>Fund Fact Sheet | Share Classes: A, C, Advisor</t>
   </si>
@@ -240,6 +237,9 @@
   </si>
   <si>
     <t>&lt;frame&gt;</t>
+  </si>
+  <si>
+    <t>{{ fund_name }}</t>
   </si>
 </sst>
 </file>
@@ -2508,10 +2508,10 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -2529,7 +2529,7 @@
     </row>
     <row r="3" spans="1:14" ht="37" x14ac:dyDescent="0.55000000000000004">
       <c r="D3" s="15" t="s">
-        <v>0</v>
+        <v>66</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="1"/>
@@ -2538,7 +2538,7 @@
       <c r="I3" s="3"/>
       <c r="J3" s="1"/>
       <c r="K3" s="21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L3" s="21"/>
       <c r="M3" s="21"/>
@@ -2598,7 +2598,7 @@
     </row>
     <row r="8" spans="1:14" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D8" s="7" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
@@ -2627,13 +2627,13 @@
     <row r="13" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
       <c r="F16" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G16" s="8"/>
       <c r="H16" s="8"/>
@@ -2646,10 +2646,10 @@
     </row>
     <row r="18" spans="1:14" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F18" s="14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G18" s="14"/>
       <c r="H18" s="14"/>
@@ -2662,21 +2662,21 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="N19" s="12"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="N19" s="12"/>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>6</v>
-      </c>
       <c r="F21" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G21" s="8"/>
       <c r="H21" s="8"/>
@@ -2689,15 +2689,15 @@
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="23" spans="1:14" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="2" t="s">
-        <v>8</v>
-      </c>
       <c r="F23" s="14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G23" s="14"/>
       <c r="H23" s="14"/>
@@ -2710,7 +2710,7 @@
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F24" s="11"/>
       <c r="G24" s="11"/>
@@ -2724,7 +2724,7 @@
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F25" s="11"/>
       <c r="G25" s="11"/>
@@ -2738,7 +2738,7 @@
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F26" s="11"/>
       <c r="G26" s="11"/>
@@ -2752,7 +2752,7 @@
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F27" s="11"/>
       <c r="G27" s="11"/>
@@ -2766,7 +2766,7 @@
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F28" s="11"/>
       <c r="G28" s="11"/>
@@ -2780,17 +2780,17 @@
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B33" s="8"/>
       <c r="C33" s="8"/>
@@ -2798,15 +2798,15 @@
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D35" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D36" s="10">
         <v>36586</v>
@@ -2814,15 +2814,15 @@
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D37" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D38" s="10">
         <v>52</v>
@@ -2830,7 +2830,7 @@
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="8"/>
@@ -2838,39 +2838,39 @@
     </row>
     <row r="42" spans="1:14" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B42" s="14"/>
       <c r="C42" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="D42" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="D42" s="17" t="s">
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A43" s="2" t="s">
+      <c r="C43" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D43" s="10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C43" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D43" s="10" t="s">
+      <c r="C44" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>35</v>
-      </c>
       <c r="D44" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F44" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G44" s="8"/>
       <c r="H44" s="8"/>
@@ -2883,27 +2883,27 @@
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D45" s="10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="C46" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D45" s="10" t="s">
+      <c r="D46" s="10" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="46" spans="1:14" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D46" s="10" t="s">
-        <v>40</v>
-      </c>
       <c r="F46" s="18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G46" s="17"/>
       <c r="H46" s="17"/>
@@ -2919,7 +2919,7 @@
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B48" s="8"/>
       <c r="C48" s="8"/>
@@ -2931,7 +2931,7 @@
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="F49" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G49" s="8"/>
       <c r="H49" s="8"/>
@@ -2947,18 +2947,18 @@
       <c r="B50" s="14"/>
       <c r="C50" s="14"/>
       <c r="D50" s="17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="51" spans="1:14" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D51" s="2">
         <v>5</v>
       </c>
       <c r="F51" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G51" s="14"/>
       <c r="H51" s="14"/>
@@ -2971,7 +2971,7 @@
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D52" s="2">
         <v>13</v>
@@ -2980,7 +2980,7 @@
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D53" s="2">
         <v>3</v>
@@ -2991,7 +2991,7 @@
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B55" s="8"/>
       <c r="C55" s="8"/>
@@ -2999,22 +2999,22 @@
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A58" s="2" t="s">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A59" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B61" s="8"/>
       <c r="C61" s="8"/>
@@ -3022,17 +3022,17 @@
     </row>
     <row r="63" spans="1:14" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B63" s="14"/>
       <c r="C63" s="14"/>
       <c r="D63" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D64" s="2">
         <v>1</v>
@@ -3040,7 +3040,7 @@
     </row>
     <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D65" s="2">
         <v>1.75</v>
@@ -3048,7 +3048,7 @@
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D66" s="2">
         <v>0.75</v>
@@ -3056,7 +3056,7 @@
     </row>
     <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B68" s="8"/>
       <c r="C68" s="8"/>
@@ -3145,10 +3145,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -3181,13 +3181,13 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" t="s">
         <v>56</v>
       </c>
-      <c r="D1" t="s">
-        <v>57</v>
-      </c>
       <c r="G1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -3198,13 +3198,13 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E2" s="13">
         <v>0.01</v>
       </c>
       <c r="G2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>